<commit_message>
Added batch logging, at least tried to fix for filtering producer-consumer interactions
Signed-off-by: kevinanewman <newman.kevin@epa.gov>
</commit_message>
<xml_diff>
--- a/input_samples/single_session_batch.xlsx
+++ b/input_samples/single_session_batch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\GitHub\EPA_OMEGA_Model\input_samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F39CA365-E399-4312-8587-4670A22BE29A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A02FCE-0883-4865-A363-40D0D8BBF343}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="405" yWindow="735" windowWidth="17625" windowHeight="16530" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="795" yWindow="735" windowWidth="17625" windowHeight="16530" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sessions" sheetId="5" r:id="rId1"/>
@@ -715,8 +715,8 @@
   <dimension ref="A1:AG44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
+      <pane ySplit="10" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
faster default single session batch...
Signed-off-by: kevinanewman <newman.kevin@epa.gov>
</commit_message>
<xml_diff>
--- a/input_samples/single_session_batch.xlsx
+++ b/input_samples/single_session_batch.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TSHERWOO\Documents\GitHub\EPA_OMEGA_Model\input_samples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\GitHub\EPA_OMEGA_Model\input_samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2EB84D7-3516-4ECA-B21A-EC4D0122B3D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59EFFE9E-8A7D-4E0F-9D96-17891FFBA064}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4500" yWindow="255" windowWidth="17955" windowHeight="16395" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sessions" sheetId="5" r:id="rId1"/>
@@ -756,23 +756,23 @@
   <dimension ref="A1:AG50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C40" sqref="C40"/>
+      <pane ySplit="10" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.44140625" style="11" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="42.42578125" style="11" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" style="1" customWidth="1"/>
     <col min="3" max="4" width="48" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="17" width="21.33203125" style="11" customWidth="1"/>
-    <col min="18" max="18" width="16.6640625" style="1" customWidth="1"/>
+    <col min="5" max="17" width="21.28515625" style="11" customWidth="1"/>
+    <col min="18" max="18" width="16.7109375" style="1" customWidth="1"/>
     <col min="19" max="19" width="18" style="1" customWidth="1"/>
-    <col min="20" max="20" width="16.44140625" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="8.6640625" style="1"/>
+    <col min="20" max="20" width="16.42578125" style="1" customWidth="1"/>
+    <col min="21" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="18" customFormat="1" ht="21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" s="18" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -813,7 +813,7 @@
       <c r="AF1" s="17"/>
       <c r="AG1" s="17"/>
     </row>
-    <row r="2" spans="1:33" s="12" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:33" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>10</v>
       </c>
@@ -833,7 +833,7 @@
       <c r="P2" s="14"/>
       <c r="Q2" s="14"/>
     </row>
-    <row r="3" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
@@ -858,7 +858,7 @@
       <c r="P3" s="14"/>
       <c r="Q3" s="14"/>
     </row>
-    <row r="4" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>27</v>
       </c>
@@ -881,7 +881,7 @@
       <c r="P4" s="14"/>
       <c r="Q4" s="14"/>
     </row>
-    <row r="5" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>28</v>
       </c>
@@ -906,7 +906,7 @@
       <c r="P5" s="14"/>
       <c r="Q5" s="14"/>
     </row>
-    <row r="6" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>50</v>
       </c>
@@ -931,7 +931,7 @@
       <c r="P6" s="14"/>
       <c r="Q6" s="14"/>
     </row>
-    <row r="7" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -949,7 +949,7 @@
       <c r="P7" s="14"/>
       <c r="Q7" s="14"/>
     </row>
-    <row r="8" spans="1:33" s="12" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:33" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>9</v>
       </c>
@@ -969,7 +969,7 @@
       <c r="P8" s="14"/>
       <c r="Q8" s="14"/>
     </row>
-    <row r="9" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>5</v>
       </c>
@@ -996,7 +996,7 @@
       <c r="R9" s="8"/>
       <c r="S9" s="8"/>
     </row>
-    <row r="10" spans="1:33" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:33" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>2</v>
       </c>
@@ -1023,7 +1023,7 @@
       <c r="R10" s="9"/>
       <c r="S10" s="9"/>
     </row>
-    <row r="11" spans="1:33" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:33" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15"/>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
@@ -1043,7 +1043,7 @@
       <c r="R11" s="14"/>
       <c r="S11" s="14"/>
     </row>
-    <row r="12" spans="1:33" s="12" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:33" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>6</v>
       </c>
@@ -1065,7 +1065,7 @@
       <c r="R12" s="14"/>
       <c r="S12" s="14"/>
     </row>
-    <row r="13" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>14</v>
       </c>
@@ -1092,7 +1092,7 @@
       <c r="R13" s="8"/>
       <c r="S13" s="8"/>
     </row>
-    <row r="14" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>16</v>
       </c>
@@ -1119,7 +1119,7 @@
       <c r="R14" s="8"/>
       <c r="S14" s="8"/>
     </row>
-    <row r="15" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>17</v>
       </c>
@@ -1146,7 +1146,7 @@
       <c r="R15" s="8"/>
       <c r="S15" s="8"/>
     </row>
-    <row r="16" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>24</v>
       </c>
@@ -1173,7 +1173,7 @@
       <c r="R16" s="8"/>
       <c r="S16" s="8"/>
     </row>
-    <row r="17" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>18</v>
       </c>
@@ -1200,7 +1200,7 @@
       <c r="R17" s="8"/>
       <c r="S17" s="8"/>
     </row>
-    <row r="18" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>49</v>
       </c>
@@ -1227,7 +1227,7 @@
       <c r="R18" s="8"/>
       <c r="S18" s="8"/>
     </row>
-    <row r="19" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>54</v>
       </c>
@@ -1254,7 +1254,7 @@
       <c r="R19" s="8"/>
       <c r="S19" s="8"/>
     </row>
-    <row r="20" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>48</v>
       </c>
@@ -1281,7 +1281,7 @@
       <c r="R20" s="8"/>
       <c r="S20" s="8"/>
     </row>
-    <row r="21" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>19</v>
       </c>
@@ -1308,7 +1308,7 @@
       <c r="R21" s="8"/>
       <c r="S21" s="8"/>
     </row>
-    <row r="22" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>20</v>
       </c>
@@ -1335,7 +1335,7 @@
       <c r="R22" s="10"/>
       <c r="S22" s="10"/>
     </row>
-    <row r="23" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>29</v>
       </c>
@@ -1362,7 +1362,7 @@
       <c r="R23" s="8"/>
       <c r="S23" s="8"/>
     </row>
-    <row r="24" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>30</v>
       </c>
@@ -1389,7 +1389,7 @@
       <c r="R24" s="8"/>
       <c r="S24" s="8"/>
     </row>
-    <row r="25" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>58</v>
       </c>
@@ -1416,7 +1416,7 @@
       <c r="R25" s="8"/>
       <c r="S25" s="8"/>
     </row>
-    <row r="26" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>59</v>
       </c>
@@ -1443,7 +1443,7 @@
       <c r="R26" s="8"/>
       <c r="S26" s="8"/>
     </row>
-    <row r="27" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>15</v>
       </c>
@@ -1470,7 +1470,7 @@
       <c r="R27" s="10"/>
       <c r="S27" s="10"/>
     </row>
-    <row r="28" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>21</v>
       </c>
@@ -1497,7 +1497,7 @@
       <c r="R28" s="8"/>
       <c r="S28" s="8"/>
     </row>
-    <row r="29" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
@@ -1514,7 +1514,7 @@
       <c r="R29" s="8"/>
       <c r="S29" s="8"/>
     </row>
-    <row r="30" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="15"/>
       <c r="C30" s="15"/>
       <c r="D30" s="15"/>
@@ -1534,7 +1534,7 @@
       <c r="R30" s="14"/>
       <c r="S30" s="14"/>
     </row>
-    <row r="31" spans="1:19" s="12" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
         <v>8</v>
       </c>
@@ -1556,7 +1556,7 @@
       <c r="R31" s="14"/>
       <c r="S31" s="14"/>
     </row>
-    <row r="32" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>45</v>
       </c>
@@ -1564,7 +1564,7 @@
         <v>13</v>
       </c>
       <c r="C32" s="8">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
@@ -1583,7 +1583,7 @@
       <c r="R32" s="8"/>
       <c r="S32" s="8"/>
     </row>
-    <row r="33" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>41</v>
       </c>
@@ -1594,7 +1594,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>42</v>
       </c>
@@ -1621,7 +1621,7 @@
       <c r="R34" s="8"/>
       <c r="S34" s="8"/>
     </row>
-    <row r="35" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
         <v>43</v>
       </c>
@@ -1629,10 +1629,10 @@
         <v>13</v>
       </c>
       <c r="C35" s="8">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="36" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>44</v>
       </c>
@@ -1659,7 +1659,7 @@
       <c r="R36" s="8"/>
       <c r="S36" s="8"/>
     </row>
-    <row r="37" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
         <v>22</v>
       </c>
@@ -1686,7 +1686,7 @@
       <c r="R37" s="10"/>
       <c r="S37" s="10"/>
     </row>
-    <row r="38" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
         <v>23</v>
       </c>
@@ -1713,7 +1713,7 @@
       <c r="R38" s="8"/>
       <c r="S38" s="8"/>
     </row>
-    <row r="39" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
         <v>31</v>
       </c>
@@ -1721,7 +1721,7 @@
         <v>11</v>
       </c>
       <c r="C39" s="8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D39" s="8"/>
       <c r="E39" s="8"/>
@@ -1740,7 +1740,7 @@
       <c r="R39" s="8"/>
       <c r="S39" s="8"/>
     </row>
-    <row r="40" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
         <v>53</v>
       </c>
@@ -1767,8 +1767,8 @@
       <c r="R40" s="8"/>
       <c r="S40" s="8"/>
     </row>
-    <row r="41" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="42" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="15"/>
       <c r="C42" s="15"/>
       <c r="D42" s="15"/>
@@ -1788,7 +1788,7 @@
       <c r="R42" s="14"/>
       <c r="S42" s="14"/>
     </row>
-    <row r="43" spans="1:19" s="12" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:19" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A43" s="20" t="s">
         <v>7</v>
       </c>
@@ -1810,7 +1810,7 @@
       <c r="R43" s="14"/>
       <c r="S43" s="14"/>
     </row>
-    <row r="44" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
         <v>60</v>
       </c>
@@ -1837,7 +1837,7 @@
       <c r="R44" s="8"/>
       <c r="S44" s="8"/>
     </row>
-    <row r="45" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
         <v>61</v>
       </c>
@@ -1864,7 +1864,7 @@
       <c r="R45" s="8"/>
       <c r="S45" s="8"/>
     </row>
-    <row r="46" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
         <v>62</v>
       </c>
@@ -1891,7 +1891,7 @@
       <c r="R46" s="8"/>
       <c r="S46" s="8"/>
     </row>
-    <row r="47" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
         <v>63</v>
       </c>
@@ -1918,7 +1918,7 @@
       <c r="R47" s="8"/>
       <c r="S47" s="8"/>
     </row>
-    <row r="48" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
         <v>64</v>
       </c>
@@ -1945,7 +1945,7 @@
       <c r="R48" s="8"/>
       <c r="S48" s="8"/>
     </row>
-    <row r="49" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
         <v>70</v>
       </c>
@@ -1972,7 +1972,7 @@
       <c r="R49" s="8"/>
       <c r="S49" s="8"/>
     </row>
-    <row r="50" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
         <v>71</v>
       </c>

</xml_diff>